<commit_message>
added test runnners and threadlocal
</commit_message>
<xml_diff>
--- a/src/resources/testdata/testdata.xlsx
+++ b/src/resources/testdata/testdata.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c03890c20013d02/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumFramework2023\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{870DD4BD-F262-4DC7-BDC7-F1F3D1047FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FCF1B7-4574-44AF-9A1C-8AE5B2252EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65B7CD18-EF92-4F6A-9D6C-EA628DEDBF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{65B7CD18-EF92-4F6A-9D6C-EA628DEDBF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
+    <sheet name="product" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>firstname</t>
   </si>
@@ -70,13 +71,43 @@
   </si>
   <si>
     <t>mitaj@123</t>
+  </si>
+  <si>
+    <t>9876778283</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>searchkey</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>expectedproductcount</t>
+  </si>
+  <si>
+    <t>macbook</t>
+  </si>
+  <si>
+    <t>MacBook Pro</t>
+  </si>
+  <si>
+    <t>MacBook Air</t>
+  </si>
+  <si>
+    <t>imac</t>
+  </si>
+  <si>
+    <t>iMac</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +119,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,11 +174,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,16 +501,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17848C2-44C0-4802-BE3F-B9D38074D9DB}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -490,8 +535,8 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>9876778283</v>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -507,8 +552,8 @@
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1">
-        <v>1234567890</v>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -524,8 +569,8 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1">
-        <v>1234567890</v>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -541,5 +586,70 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{44083D29-1F82-4F4F-9A9C-CD1D1A375FDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0D77F6-EF37-4BB6-89A9-595ADA7DD478}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>